<commit_message>
CONEXION CON EL FRONT
</commit_message>
<xml_diff>
--- a/Archivo de prueba reels para Niyi.xlsx
+++ b/Archivo de prueba reels para Niyi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESARROLLADOR\Documents\Manuel Cardona\bot_reels_excel_communitys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Programador2\Documents\Antonio Barreto\Communitys\bot_reels_excel_communitys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F835B397-C1F6-4726-901A-06293B43748C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59637E22-7451-4E4D-8067-424D01E2AC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="58">
   <si>
     <t>Text</t>
   </si>
@@ -187,16 +187,10 @@
     <t>05:24:00 PM</t>
   </si>
   <si>
-    <t>SHORT</t>
-  </si>
-  <si>
     <t>PUBLIC</t>
   </si>
   <si>
     <t>ENTERTAINMENT</t>
-  </si>
-  <si>
-    <t>REEL</t>
   </si>
   <si>
     <t>PUBLIC_TO_EVERYONE</t>
@@ -524,14 +518,15 @@
   </sheetPr>
   <dimension ref="A1:BD998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="35" max="35" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="38.25" x14ac:dyDescent="0.2">
@@ -710,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="10" t="b">
         <v>0</v>
@@ -722,16 +717,16 @@
         <v>0</v>
       </c>
       <c r="I2" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K2" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="12" t="b">
         <v>0</v>
@@ -756,28 +751,22 @@
       <c r="AC2" s="14"/>
       <c r="AD2" s="14"/>
       <c r="AE2" s="14"/>
-      <c r="AF2" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF2" s="5"/>
       <c r="AG2" s="14"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK2" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM2" s="2"/>
       <c r="AN2" s="14"/>
-      <c r="AO2" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO2" s="5"/>
       <c r="AP2" s="6"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
@@ -791,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="AV2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW2" s="15" t="b">
         <v>0</v>
@@ -818,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="10" t="b">
         <v>0</v>
@@ -830,16 +819,16 @@
         <v>0</v>
       </c>
       <c r="I3" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K3" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="12" t="b">
         <v>0</v>
@@ -864,28 +853,22 @@
       <c r="AC3" s="14"/>
       <c r="AD3" s="14"/>
       <c r="AE3" s="14"/>
-      <c r="AF3" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF3" s="5"/>
       <c r="AG3" s="14"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="3" t="s">
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK3" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM3" s="2"/>
       <c r="AN3" s="14"/>
-      <c r="AO3" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO3" s="5"/>
       <c r="AP3" s="6"/>
       <c r="AQ3" s="2"/>
       <c r="AR3" s="2"/>
@@ -899,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="AV3" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW3" s="15" t="b">
         <v>0</v>
@@ -926,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="10" t="b">
         <v>0</v>
@@ -938,16 +921,16 @@
         <v>0</v>
       </c>
       <c r="I4" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K4" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="12" t="b">
         <v>0</v>
@@ -972,28 +955,22 @@
       <c r="AC4" s="14"/>
       <c r="AD4" s="14"/>
       <c r="AE4" s="14"/>
-      <c r="AF4" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF4" s="5"/>
       <c r="AG4" s="14"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="3" t="s">
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK4" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM4" s="2"/>
       <c r="AN4" s="14"/>
-      <c r="AO4" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO4" s="5"/>
       <c r="AP4" s="6"/>
       <c r="AQ4" s="2"/>
       <c r="AR4" s="2"/>
@@ -1007,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="AV4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW4" s="15" t="b">
         <v>0</v>
@@ -1034,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="10" t="b">
         <v>0</v>
@@ -1046,16 +1023,16 @@
         <v>0</v>
       </c>
       <c r="I5" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K5" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="12" t="b">
         <v>0</v>
@@ -1080,28 +1057,22 @@
       <c r="AC5" s="14"/>
       <c r="AD5" s="14"/>
       <c r="AE5" s="14"/>
-      <c r="AF5" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF5" s="5"/>
       <c r="AG5" s="14"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="3" t="s">
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ5" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK5" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM5" s="2"/>
       <c r="AN5" s="14"/>
-      <c r="AO5" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO5" s="5"/>
       <c r="AP5" s="6"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
@@ -1115,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW5" s="15" t="b">
         <v>0</v>
@@ -1142,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="10" t="b">
         <v>0</v>
@@ -1154,16 +1125,16 @@
         <v>0</v>
       </c>
       <c r="I6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="12" t="b">
         <v>0</v>
@@ -1188,28 +1159,22 @@
       <c r="AC6" s="14"/>
       <c r="AD6" s="14"/>
       <c r="AE6" s="14"/>
-      <c r="AF6" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF6" s="5"/>
       <c r="AG6" s="14"/>
       <c r="AH6" s="2"/>
-      <c r="AI6" s="3" t="s">
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK6" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="14"/>
-      <c r="AO6" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO6" s="5"/>
       <c r="AP6" s="6"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
@@ -1223,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW6" s="15" t="b">
         <v>0</v>
@@ -1250,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="10" t="b">
         <v>0</v>
@@ -1262,16 +1227,16 @@
         <v>0</v>
       </c>
       <c r="I7" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K7" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="12" t="b">
         <v>0</v>
@@ -1296,28 +1261,22 @@
       <c r="AC7" s="14"/>
       <c r="AD7" s="14"/>
       <c r="AE7" s="14"/>
-      <c r="AF7" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF7" s="5"/>
       <c r="AG7" s="14"/>
       <c r="AH7" s="2"/>
-      <c r="AI7" s="3" t="s">
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ7" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK7" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM7" s="2"/>
       <c r="AN7" s="14"/>
-      <c r="AO7" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO7" s="5"/>
       <c r="AP7" s="6"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
@@ -1331,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="AV7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW7" s="15" t="b">
         <v>0</v>
@@ -1358,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="10" t="b">
         <v>0</v>
@@ -1370,16 +1329,16 @@
         <v>0</v>
       </c>
       <c r="I8" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K8" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="12" t="b">
         <v>0</v>
@@ -1404,28 +1363,22 @@
       <c r="AC8" s="14"/>
       <c r="AD8" s="14"/>
       <c r="AE8" s="14"/>
-      <c r="AF8" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF8" s="5"/>
       <c r="AG8" s="14"/>
       <c r="AH8" s="2"/>
-      <c r="AI8" s="3" t="s">
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK8" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM8" s="2"/>
       <c r="AN8" s="14"/>
-      <c r="AO8" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO8" s="5"/>
       <c r="AP8" s="6"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
@@ -1439,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="AV8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW8" s="15" t="b">
         <v>0</v>
@@ -1466,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="10" t="b">
         <v>0</v>
@@ -1478,16 +1431,16 @@
         <v>0</v>
       </c>
       <c r="I9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="12" t="b">
         <v>0</v>
@@ -1512,28 +1465,22 @@
       <c r="AC9" s="14"/>
       <c r="AD9" s="14"/>
       <c r="AE9" s="14"/>
-      <c r="AF9" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF9" s="5"/>
       <c r="AG9" s="14"/>
       <c r="AH9" s="2"/>
-      <c r="AI9" s="3" t="s">
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ9" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK9" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM9" s="2"/>
       <c r="AN9" s="14"/>
-      <c r="AO9" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO9" s="5"/>
       <c r="AP9" s="6"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
@@ -1547,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="AV9" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW9" s="15" t="b">
         <v>0</v>
@@ -1574,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>0</v>
@@ -1586,16 +1533,16 @@
         <v>0</v>
       </c>
       <c r="I10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="12" t="b">
         <v>0</v>
@@ -1620,28 +1567,22 @@
       <c r="AC10" s="14"/>
       <c r="AD10" s="14"/>
       <c r="AE10" s="14"/>
-      <c r="AF10" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF10" s="5"/>
       <c r="AG10" s="14"/>
       <c r="AH10" s="2"/>
-      <c r="AI10" s="3" t="s">
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ10" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK10" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM10" s="2"/>
       <c r="AN10" s="14"/>
-      <c r="AO10" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO10" s="5"/>
       <c r="AP10" s="6"/>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2"/>
@@ -1655,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="AV10" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW10" s="15" t="b">
         <v>0</v>
@@ -1682,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="10" t="b">
         <v>0</v>
@@ -1694,16 +1635,16 @@
         <v>0</v>
       </c>
       <c r="I11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="12" t="b">
         <v>0</v>
@@ -1728,28 +1669,22 @@
       <c r="AC11" s="14"/>
       <c r="AD11" s="14"/>
       <c r="AE11" s="14"/>
-      <c r="AF11" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF11" s="5"/>
       <c r="AG11" s="14"/>
       <c r="AH11" s="2"/>
-      <c r="AI11" s="3" t="s">
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK11" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM11" s="2"/>
       <c r="AN11" s="14"/>
-      <c r="AO11" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO11" s="5"/>
       <c r="AP11" s="6"/>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
@@ -1763,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="AV11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW11" s="15" t="b">
         <v>0</v>
@@ -1790,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="10" t="b">
         <v>0</v>
@@ -1802,16 +1737,16 @@
         <v>0</v>
       </c>
       <c r="I12" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K12" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="12" t="b">
         <v>0</v>
@@ -1836,28 +1771,22 @@
       <c r="AC12" s="14"/>
       <c r="AD12" s="14"/>
       <c r="AE12" s="14"/>
-      <c r="AF12" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF12" s="5"/>
       <c r="AG12" s="14"/>
       <c r="AH12" s="2"/>
-      <c r="AI12" s="3" t="s">
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ12" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK12" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM12" s="2"/>
       <c r="AN12" s="14"/>
-      <c r="AO12" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO12" s="5"/>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
@@ -1871,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="AV12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW12" s="15" t="b">
         <v>0</v>
@@ -1898,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="10" t="b">
         <v>0</v>
@@ -1910,16 +1839,16 @@
         <v>0</v>
       </c>
       <c r="I13" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K13" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="12" t="b">
         <v>0</v>
@@ -1944,28 +1873,22 @@
       <c r="AC13" s="14"/>
       <c r="AD13" s="14"/>
       <c r="AE13" s="14"/>
-      <c r="AF13" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF13" s="5"/>
       <c r="AG13" s="14"/>
       <c r="AH13" s="2"/>
-      <c r="AI13" s="3" t="s">
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ13" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK13" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM13" s="2"/>
       <c r="AN13" s="14"/>
-      <c r="AO13" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO13" s="5"/>
       <c r="AP13" s="6"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
@@ -1979,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW13" s="15" t="b">
         <v>0</v>
@@ -2006,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="10" t="b">
         <v>0</v>
@@ -2018,16 +1941,16 @@
         <v>0</v>
       </c>
       <c r="I14" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K14" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="12" t="b">
         <v>0</v>
@@ -2052,28 +1975,22 @@
       <c r="AC14" s="14"/>
       <c r="AD14" s="14"/>
       <c r="AE14" s="14"/>
-      <c r="AF14" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF14" s="5"/>
       <c r="AG14" s="14"/>
       <c r="AH14" s="2"/>
-      <c r="AI14" s="3" t="s">
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK14" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL14" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM14" s="2"/>
       <c r="AN14" s="14"/>
-      <c r="AO14" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO14" s="5"/>
       <c r="AP14" s="6"/>
       <c r="AQ14" s="2"/>
       <c r="AR14" s="2"/>
@@ -2087,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW14" s="15" t="b">
         <v>0</v>
@@ -2114,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="10" t="b">
         <v>0</v>
@@ -2126,16 +2043,16 @@
         <v>0</v>
       </c>
       <c r="I15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="12" t="b">
         <v>0</v>
@@ -2160,28 +2077,22 @@
       <c r="AC15" s="14"/>
       <c r="AD15" s="14"/>
       <c r="AE15" s="14"/>
-      <c r="AF15" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF15" s="5"/>
       <c r="AG15" s="14"/>
       <c r="AH15" s="2"/>
-      <c r="AI15" s="3" t="s">
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ15" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK15" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="14"/>
-      <c r="AO15" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO15" s="5"/>
       <c r="AP15" s="6"/>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2"/>
@@ -2195,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="AV15" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW15" s="15" t="b">
         <v>0</v>
@@ -2222,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="10" t="b">
         <v>0</v>
@@ -2234,16 +2145,16 @@
         <v>0</v>
       </c>
       <c r="I16" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K16" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="12" t="b">
         <v>0</v>
@@ -2268,28 +2179,22 @@
       <c r="AC16" s="14"/>
       <c r="AD16" s="14"/>
       <c r="AE16" s="14"/>
-      <c r="AF16" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF16" s="5"/>
       <c r="AG16" s="14"/>
       <c r="AH16" s="2"/>
-      <c r="AI16" s="3" t="s">
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ16" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK16" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM16" s="2"/>
       <c r="AN16" s="14"/>
-      <c r="AO16" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO16" s="5"/>
       <c r="AP16" s="6"/>
       <c r="AQ16" s="2"/>
       <c r="AR16" s="2"/>
@@ -2303,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="AV16" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW16" s="15" t="b">
         <v>0</v>
@@ -2330,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="10" t="b">
         <v>0</v>
@@ -2342,16 +2247,16 @@
         <v>0</v>
       </c>
       <c r="I17" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K17" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="12" t="b">
         <v>0</v>
@@ -2376,28 +2281,22 @@
       <c r="AC17" s="14"/>
       <c r="AD17" s="14"/>
       <c r="AE17" s="14"/>
-      <c r="AF17" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF17" s="5"/>
       <c r="AG17" s="14"/>
       <c r="AH17" s="2"/>
-      <c r="AI17" s="3" t="s">
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ17" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK17" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM17" s="2"/>
       <c r="AN17" s="14"/>
-      <c r="AO17" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO17" s="5"/>
       <c r="AP17" s="6"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
@@ -2411,7 +2310,7 @@
         <v>0</v>
       </c>
       <c r="AV17" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW17" s="15" t="b">
         <v>0</v>
@@ -2438,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="10" t="b">
         <v>0</v>
@@ -2450,16 +2349,16 @@
         <v>0</v>
       </c>
       <c r="I18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="12" t="b">
         <v>0</v>
@@ -2484,28 +2383,22 @@
       <c r="AC18" s="14"/>
       <c r="AD18" s="14"/>
       <c r="AE18" s="14"/>
-      <c r="AF18" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF18" s="5"/>
       <c r="AG18" s="14"/>
       <c r="AH18" s="2"/>
-      <c r="AI18" s="3" t="s">
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ18" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK18" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM18" s="2"/>
       <c r="AN18" s="14"/>
-      <c r="AO18" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO18" s="5"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="2"/>
@@ -2519,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW18" s="15" t="b">
         <v>0</v>
@@ -2546,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="10" t="b">
         <v>0</v>
@@ -2558,16 +2451,16 @@
         <v>0</v>
       </c>
       <c r="I19" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K19" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="12" t="b">
         <v>0</v>
@@ -2592,28 +2485,22 @@
       <c r="AC19" s="14"/>
       <c r="AD19" s="14"/>
       <c r="AE19" s="14"/>
-      <c r="AF19" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF19" s="5"/>
       <c r="AG19" s="14"/>
       <c r="AH19" s="2"/>
-      <c r="AI19" s="3" t="s">
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ19" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK19" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="14"/>
-      <c r="AO19" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO19" s="5"/>
       <c r="AP19" s="6"/>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
@@ -2627,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="AV19" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW19" s="15" t="b">
         <v>0</v>
@@ -2654,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="10" t="b">
         <v>0</v>
@@ -2666,16 +2553,16 @@
         <v>0</v>
       </c>
       <c r="I20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" s="12" t="b">
         <v>0</v>
@@ -2700,28 +2587,22 @@
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
       <c r="AE20" s="14"/>
-      <c r="AF20" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF20" s="5"/>
       <c r="AG20" s="14"/>
       <c r="AH20" s="2"/>
-      <c r="AI20" s="3" t="s">
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ20" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK20" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM20" s="2"/>
       <c r="AN20" s="14"/>
-      <c r="AO20" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO20" s="5"/>
       <c r="AP20" s="6"/>
       <c r="AQ20" s="2"/>
       <c r="AR20" s="2"/>
@@ -2735,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="AV20" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW20" s="15" t="b">
         <v>0</v>
@@ -2762,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="10" t="b">
         <v>0</v>
@@ -2774,16 +2655,16 @@
         <v>0</v>
       </c>
       <c r="I21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="12" t="b">
         <v>0</v>
@@ -2808,28 +2689,22 @@
       <c r="AC21" s="14"/>
       <c r="AD21" s="14"/>
       <c r="AE21" s="14"/>
-      <c r="AF21" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF21" s="5"/>
       <c r="AG21" s="14"/>
       <c r="AH21" s="2"/>
-      <c r="AI21" s="3" t="s">
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ21" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK21" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM21" s="2"/>
       <c r="AN21" s="14"/>
-      <c r="AO21" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO21" s="5"/>
       <c r="AP21" s="6"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
@@ -2843,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="AV21" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW21" s="15" t="b">
         <v>0</v>
@@ -2870,7 +2745,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="10" t="b">
         <v>0</v>
@@ -2882,16 +2757,16 @@
         <v>0</v>
       </c>
       <c r="I22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="12" t="b">
         <v>0</v>
@@ -2916,28 +2791,22 @@
       <c r="AC22" s="14"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
-      <c r="AF22" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF22" s="5"/>
       <c r="AG22" s="14"/>
       <c r="AH22" s="2"/>
-      <c r="AI22" s="3" t="s">
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ22" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK22" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM22" s="2"/>
       <c r="AN22" s="14"/>
-      <c r="AO22" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO22" s="5"/>
       <c r="AP22" s="6"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2"/>
@@ -2951,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="AV22" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW22" s="15" t="b">
         <v>0</v>
@@ -2978,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="10" t="b">
         <v>0</v>
@@ -2990,16 +2859,16 @@
         <v>0</v>
       </c>
       <c r="I23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="12" t="b">
         <v>0</v>
@@ -3024,28 +2893,22 @@
       <c r="AC23" s="14"/>
       <c r="AD23" s="14"/>
       <c r="AE23" s="14"/>
-      <c r="AF23" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF23" s="5"/>
       <c r="AG23" s="14"/>
       <c r="AH23" s="2"/>
-      <c r="AI23" s="3" t="s">
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ23" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK23" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="14"/>
-      <c r="AO23" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO23" s="5"/>
       <c r="AP23" s="6"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2"/>
@@ -3059,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="AV23" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW23" s="15" t="b">
         <v>0</v>
@@ -3086,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="10" t="b">
         <v>0</v>
@@ -3098,16 +2961,16 @@
         <v>0</v>
       </c>
       <c r="I24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="12" t="b">
         <v>0</v>
@@ -3132,28 +2995,22 @@
       <c r="AC24" s="14"/>
       <c r="AD24" s="14"/>
       <c r="AE24" s="14"/>
-      <c r="AF24" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF24" s="5"/>
       <c r="AG24" s="14"/>
       <c r="AH24" s="2"/>
-      <c r="AI24" s="3" t="s">
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ24" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK24" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM24" s="2"/>
       <c r="AN24" s="14"/>
-      <c r="AO24" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO24" s="5"/>
       <c r="AP24" s="6"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
@@ -3167,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="AV24" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW24" s="15" t="b">
         <v>0</v>
@@ -3194,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="10" t="b">
         <v>0</v>
@@ -3206,16 +3063,16 @@
         <v>0</v>
       </c>
       <c r="I25" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K25" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="12" t="b">
         <v>0</v>
@@ -3240,28 +3097,22 @@
       <c r="AC25" s="14"/>
       <c r="AD25" s="14"/>
       <c r="AE25" s="14"/>
-      <c r="AF25" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF25" s="5"/>
       <c r="AG25" s="14"/>
       <c r="AH25" s="2"/>
-      <c r="AI25" s="3" t="s">
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ25" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK25" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM25" s="2"/>
       <c r="AN25" s="14"/>
-      <c r="AO25" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO25" s="5"/>
       <c r="AP25" s="6"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
@@ -3275,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="AV25" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW25" s="15" t="b">
         <v>0</v>
@@ -3302,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="10" t="b">
         <v>0</v>
@@ -3314,16 +3165,16 @@
         <v>0</v>
       </c>
       <c r="I26" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K26" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="12" t="b">
         <v>0</v>
@@ -3348,28 +3199,22 @@
       <c r="AC26" s="14"/>
       <c r="AD26" s="14"/>
       <c r="AE26" s="14"/>
-      <c r="AF26" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF26" s="5"/>
       <c r="AG26" s="14"/>
       <c r="AH26" s="2"/>
-      <c r="AI26" s="3" t="s">
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ26" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK26" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM26" s="2"/>
       <c r="AN26" s="14"/>
-      <c r="AO26" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO26" s="5"/>
       <c r="AP26" s="6"/>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
@@ -3383,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="AV26" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW26" s="15" t="b">
         <v>0</v>
@@ -3410,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="10" t="b">
         <v>0</v>
@@ -3422,16 +3267,16 @@
         <v>0</v>
       </c>
       <c r="I27" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K27" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="12" t="b">
         <v>0</v>
@@ -3456,28 +3301,22 @@
       <c r="AC27" s="14"/>
       <c r="AD27" s="14"/>
       <c r="AE27" s="14"/>
-      <c r="AF27" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF27" s="5"/>
       <c r="AG27" s="14"/>
       <c r="AH27" s="2"/>
-      <c r="AI27" s="3" t="s">
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ27" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK27" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="14"/>
-      <c r="AO27" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO27" s="5"/>
       <c r="AP27" s="6"/>
       <c r="AQ27" s="2"/>
       <c r="AR27" s="2"/>
@@ -3491,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="AV27" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW27" s="15" t="b">
         <v>0</v>
@@ -3518,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="10" t="b">
         <v>0</v>
@@ -3530,16 +3369,16 @@
         <v>0</v>
       </c>
       <c r="I28" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K28" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="12" t="b">
         <v>0</v>
@@ -3564,28 +3403,22 @@
       <c r="AC28" s="14"/>
       <c r="AD28" s="14"/>
       <c r="AE28" s="14"/>
-      <c r="AF28" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF28" s="5"/>
       <c r="AG28" s="14"/>
       <c r="AH28" s="2"/>
-      <c r="AI28" s="3" t="s">
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ28" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK28" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM28" s="2"/>
       <c r="AN28" s="14"/>
-      <c r="AO28" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO28" s="5"/>
       <c r="AP28" s="6"/>
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
@@ -3599,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="AV28" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW28" s="15" t="b">
         <v>0</v>
@@ -3626,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="10" t="b">
         <v>0</v>
@@ -3638,16 +3471,16 @@
         <v>0</v>
       </c>
       <c r="I29" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K29" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="12" t="b">
         <v>0</v>
@@ -3672,28 +3505,22 @@
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
-      <c r="AF29" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF29" s="5"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
-      <c r="AI29" s="3" t="s">
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ29" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK29" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL29" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
-      <c r="AO29" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO29" s="5"/>
       <c r="AP29" s="6"/>
       <c r="AQ29" s="2"/>
       <c r="AR29" s="2"/>
@@ -3707,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="AV29" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW29" s="15" t="b">
         <v>0</v>
@@ -3734,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="10" t="b">
         <v>0</v>
@@ -3746,16 +3573,16 @@
         <v>0</v>
       </c>
       <c r="I30" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K30" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="12" t="b">
         <v>0</v>
@@ -3780,28 +3607,22 @@
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
-      <c r="AF30" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF30" s="5"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
-      <c r="AI30" s="3" t="s">
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ30" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK30" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL30" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
-      <c r="AO30" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO30" s="5"/>
       <c r="AP30" s="6"/>
       <c r="AQ30" s="2"/>
       <c r="AR30" s="2"/>
@@ -3815,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="AV30" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW30" s="15" t="b">
         <v>0</v>
@@ -3842,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="10" t="b">
         <v>0</v>
@@ -3854,16 +3675,16 @@
         <v>0</v>
       </c>
       <c r="I31" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="10" t="b">
         <v>0</v>
       </c>
       <c r="K31" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="12" t="b">
         <v>0</v>
@@ -3888,28 +3709,22 @@
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
-      <c r="AF31" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AF31" s="5"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
-      <c r="AI31" s="3" t="s">
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ31" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="AK31" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AL31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
-      <c r="AO31" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="AO31" s="5"/>
       <c r="AP31" s="6"/>
       <c r="AQ31" s="2"/>
       <c r="AR31" s="2"/>
@@ -3923,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="AV31" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AW31" s="15" t="b">
         <v>0</v>

</xml_diff>